<commit_message>
fix in template Fix project selection
</commit_message>
<xml_diff>
--- a/CommitmentLettersApp/ImportTemplates/תבנית יבוא התחיבויות.xlsx
+++ b/CommitmentLettersApp/ImportTemplates/תבנית יבוא התחיבויות.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DrLogyMisc\CommitmentLettersApp\ImportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88FC356-A744-4445-829D-02FD70AF4330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AC9521-55DB-4B95-8FFF-9873C6CA6007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{80D5FA03-17CC-472B-A333-F3A10A5D6810}"/>
   </bookViews>
@@ -636,7 +636,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -644,7 +644,7 @@
     <col min="2" max="2" width="8.6640625" style="3"/>
     <col min="3" max="3" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="5" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" style="8"/>
     <col min="8" max="8" width="9.4140625" style="8" bestFit="1" customWidth="1"/>
@@ -767,12 +767,12 @@
   <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B4128A4-7196-4215-9F67-B22DDA4A1998}">
           <x14:formula1>
             <xm:f>טבלאות!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:F6</xm:sqref>
+          <xm:sqref>E2:E6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1728F99E-8A96-44F6-B0A5-176E6F345F24}">
           <x14:formula1>

</xml_diff>

<commit_message>
commitment letters bug fixes pdfmailer - support archive
</commit_message>
<xml_diff>
--- a/CommitmentLettersApp/ImportTemplates/תבנית יבוא התחיבויות.xlsx
+++ b/CommitmentLettersApp/ImportTemplates/תבנית יבוא התחיבויות.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DrLogyMisc\CommitmentLettersApp\ImportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FE8EBE-C4DF-4076-A309-F293B587EFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20200543-D0B4-4DFB-8081-DA9C46E20A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{80D5FA03-17CC-472B-A333-F3A10A5D6810}"/>
   </bookViews>
@@ -639,7 +639,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -648,7 +648,7 @@
     <col min="3" max="3" width="11" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.75" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" style="8"/>
     <col min="8" max="8" width="9.4140625" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
@@ -675,7 +675,7 @@
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -770,7 +770,7 @@
   <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B4128A4-7196-4215-9F67-B22DDA4A1998}">
           <x14:formula1>
             <xm:f>טבלאות!$A$2:$A$9</xm:f>

</xml_diff>